<commit_message>
adjusted the scanners in Main to all use 1 single scanner - needed to use BufferedInput import to make this work
Added Passwords
- Adjusted login to be from the Security folder
</commit_message>
<xml_diff>
--- a/data/ApplicantList.xlsx
+++ b/data/ApplicantList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/hu0037ng_e_ntu_edu_sg/Documents/SC4079 - Final Year Project/SC2002/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyeyo\SC2002-Group-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC1048D321184AB85ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E7B5106-FDD2-4501-9B14-A9486EC70E42}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDF4C5F-4FD4-471C-B419-D9C2CC02EE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13296" yWindow="2376" windowWidth="9744" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,12 +399,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -438,7 +438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -455,7 +455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -472,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -489,7 +489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>

</xml_diff>